<commit_message>
update some experiments and plot function
</commit_message>
<xml_diff>
--- a/SWIQuant-Part2/TestResult5000/记录.xlsx
+++ b/SWIQuant-Part2/TestResult5000/记录.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yyy96\Documents\VScodework\SWI_Quantification_network\SWIQuant-Part2\TestResult5000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E9657F-180C-4CE1-BDC2-0BE4EAE27A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502F5102-4156-4BCB-9807-A6F8F7B05167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 

</xml_diff>